<commit_message>
Se agrega la question para la transaccion carga ePrepago con cuenta de ahorro en cero
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\e-prepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\eprepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF7C08A-80AE-437C-931E-E40E016E970E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54256902-CFCE-42A6-8ACC-46C6A01D1E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A4" sqref="A4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -602,7 +602,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.5">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>93221453</v>
@@ -646,6 +646,23 @@
       <c r="O3" s="3" t="s">
         <v>26</v>
       </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.5">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
recarga eprepago escenarios alternos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\eprepago\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\eprepago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54256902-CFCE-42A6-8ACC-46C6A01D1E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="2265" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="CargaSobreMaximo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -106,19 +104,34 @@
     <t>406-714500-19</t>
   </si>
   <si>
-    <t>autotest28</t>
-  </si>
-  <si>
-    <t>406-714530-16</t>
-  </si>
-  <si>
     <t>10000</t>
+  </si>
+  <si>
+    <t>autotest30</t>
+  </si>
+  <si>
+    <t>406-733020-15</t>
+  </si>
+  <si>
+    <t>406-733020-16</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>406-733020-17</t>
+  </si>
+  <si>
+    <t>Alterno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -491,22 +504,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:P4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -600,7 +617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.5">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -611,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3">
         <v>1234</v>
@@ -620,7 +637,7 @@
         <v>4321</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -638,46 +655,111 @@
         <v>17</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>93221453</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="E4" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="15.5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+    <row r="5" spans="1:15" ht="15.75">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>93221453</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
escenarios alternos carga eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/eprepago/recargar_tarjeta_virtual_eprepago.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Ahorros</t>
   </si>
   <si>
-    <t>autotest25</t>
-  </si>
-  <si>
-    <t>1000000</t>
-  </si>
-  <si>
     <t>406-714500-19</t>
   </si>
   <si>
@@ -119,13 +113,22 @@
     <t>2000000</t>
   </si>
   <si>
-    <t>25000</t>
-  </si>
-  <si>
-    <t>406-733020-17</t>
-  </si>
-  <si>
     <t>Alterno</t>
+  </si>
+  <si>
+    <t>406-733020-18</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>406-733020-19</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>160000</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -581,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3">
         <v>1234</v>
@@ -608,13 +611,13 @@
         <v>17</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75">
@@ -628,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3">
         <v>1234</v>
@@ -637,7 +640,7 @@
         <v>4321</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -655,13 +658,13 @@
         <v>17</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75">
@@ -675,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3">
         <v>1234</v>
@@ -684,7 +687,7 @@
         <v>4321</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>13</v>
@@ -702,13 +705,13 @@
         <v>17</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
@@ -722,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>1234</v>
@@ -731,7 +734,7 @@
         <v>4321</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
@@ -755,6 +758,53 @@
         <v>21</v>
       </c>
       <c r="O5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>93221453</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>